<commit_message>
temporary change to account 4049; temporarily needs to be 4046
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\01_Dave\Programs\GitHub_home\budget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378EE056-3775-48BD-B9B7-51E43BB20C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608AE6B0-4CE0-4DD3-A325-84B74BD0A824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -974,22 +974,22 @@
     <t>4000 Classis Assessment</t>
   </si>
   <si>
+    <t>InOrOut</t>
+  </si>
+  <si>
+    <t>GreenSheet</t>
+  </si>
+  <si>
+    <t>Committee</t>
+  </si>
+  <si>
+    <t>SourceOfFunds</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
     <t>4046 UP Mission Fund Income</t>
-  </si>
-  <si>
-    <t>InOrOut</t>
-  </si>
-  <si>
-    <t>GreenSheet</t>
-  </si>
-  <si>
-    <t>Committee</t>
-  </si>
-  <si>
-    <t>SourceOfFunds</t>
-  </si>
-  <si>
-    <t>Account</t>
   </si>
 </sst>
 </file>
@@ -4949,9 +4949,9 @@
   <dimension ref="A1:L224"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L17" sqref="L17"/>
-      <selection pane="bottomLeft" activeCell="K182" sqref="K182:K185"/>
+      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4971,22 +4971,22 @@
   <sheetData>
     <row r="1" spans="1:12" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>293</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>300</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>301</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>212</v>
@@ -6942,7 +6942,7 @@
         <v>22</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>222</v>

</xml_diff>